<commit_message>
file cleanup, added versioning
</commit_message>
<xml_diff>
--- a/My-Trading-Journal-Template.xlsx
+++ b/My-Trading-Journal-Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\TradeJournal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB6A77D-7680-44AE-AAE5-6923C18C5BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7966D1A-AA65-42C7-9EBA-28FD111891D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -152,9 +152,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -212,9 +211,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,9 +518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -548,10 +545,10 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -592,7 +589,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -623,7 +620,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -636,7 +633,7 @@
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -650,7 +647,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -689,7 +686,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -767,18 +764,18 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.08984375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="2" t="s">

</xml_diff>

<commit_message>
fixed parsing, reformated xls, data mapping finalized
</commit_message>
<xml_diff>
--- a/My-Trading-Journal-Template.xlsx
+++ b/My-Trading-Journal-Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\TradeJournal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7966D1A-AA65-42C7-9EBA-28FD111891D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DC8744-9427-4FB7-9B7D-7033FA6D1AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -40,6 +40,9 @@
     <t>Ticker Symbol</t>
   </si>
   <si>
+    <t>Shares</t>
+  </si>
+  <si>
     <t>Position Size</t>
   </si>
   <si>
@@ -55,6 +58,57 @@
     <t>Long/Short</t>
   </si>
   <si>
+    <t>09/03/2024</t>
+  </si>
+  <si>
+    <t>AUUD</t>
+  </si>
+  <si>
+    <t>Sell</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Buy</t>
+  </si>
+  <si>
+    <t>MDB</t>
+  </si>
+  <si>
+    <t>09/04/2024</t>
+  </si>
+  <si>
+    <t>09/05/2024</t>
+  </si>
+  <si>
+    <t>TWFG</t>
+  </si>
+  <si>
+    <t>09/09/2024</t>
+  </si>
+  <si>
+    <t>SMMT</t>
+  </si>
+  <si>
+    <t>09/25/2024</t>
+  </si>
+  <si>
+    <t>BNZI</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>09/26/2024</t>
+  </si>
+  <si>
+    <t>TBIO</t>
+  </si>
+  <si>
+    <t>KTTA</t>
+  </si>
+  <si>
     <t>Stop-Loss Level</t>
   </si>
   <si>
@@ -68,6 +122,12 @@
   </si>
   <si>
     <t>Commissions and Fees</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>Net</t>
   </si>
   <si>
     <t>Market Context</t>
@@ -152,8 +212,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  <numFmts count="3">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -207,13 +269,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="46" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,46 +584,879 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>86</v>
+      </c>
+      <c r="E2" s="11">
+        <v>99.77</v>
+      </c>
+      <c r="G2" s="9">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>86</v>
+      </c>
+      <c r="E3" s="11">
+        <v>99.76</v>
+      </c>
+      <c r="F3" s="11">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>0.34900999999999999</v>
+      </c>
+      <c r="E4" s="11">
+        <v>100</v>
+      </c>
+      <c r="F4" s="11">
+        <v>286.52</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>0.34900999999999999</v>
+      </c>
+      <c r="E5" s="11">
+        <v>101.47</v>
+      </c>
+      <c r="G5" s="9">
+        <v>290.73</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6" s="11">
+        <v>248.3</v>
+      </c>
+      <c r="F6" s="11">
+        <v>31.04</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7" s="11">
+        <v>267.95999999999998</v>
+      </c>
+      <c r="G7" s="9">
+        <v>19.14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>27</v>
+      </c>
+      <c r="E8" s="11">
+        <v>500.31</v>
+      </c>
+      <c r="G8" s="9">
+        <v>18.53</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>27</v>
+      </c>
+      <c r="E9" s="11">
+        <v>495.99</v>
+      </c>
+      <c r="F9" s="11">
+        <v>18.37</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10" s="11">
+        <v>236.04</v>
+      </c>
+      <c r="F10" s="11">
+        <v>16.86</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>17</v>
+      </c>
+      <c r="E11" s="11">
+        <v>98.6</v>
+      </c>
+      <c r="F11" s="11">
+        <v>5.8</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="11">
+        <v>94.61</v>
+      </c>
+      <c r="F12" s="11">
+        <v>94.61</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="11">
+        <v>94.98</v>
+      </c>
+      <c r="G13" s="9">
+        <v>94.98</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14">
+        <v>17</v>
+      </c>
+      <c r="E14" s="11">
+        <v>102.34</v>
+      </c>
+      <c r="G14" s="9">
+        <v>6.02</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>86</v>
+      </c>
+      <c r="E15">
+        <v>99.77</v>
+      </c>
+      <c r="F15"/>
+      <c r="G15">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>86</v>
+      </c>
+      <c r="E16">
+        <v>99.76</v>
+      </c>
+      <c r="F16">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="G16"/>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17">
+        <v>0.34900999999999999</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="F17">
+        <v>286.52</v>
+      </c>
+      <c r="G17"/>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>0.34900999999999999</v>
+      </c>
+      <c r="E18">
+        <v>101.47</v>
+      </c>
+      <c r="F18"/>
+      <c r="G18">
+        <v>290.73</v>
+      </c>
+      <c r="H18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <v>248.3</v>
+      </c>
+      <c r="F19">
+        <v>31.04</v>
+      </c>
+      <c r="G19"/>
+      <c r="H19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>14</v>
+      </c>
+      <c r="E20">
+        <v>267.95999999999998</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20">
+        <v>19.14</v>
+      </c>
+      <c r="H20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>27</v>
+      </c>
+      <c r="E21">
+        <v>500.31</v>
+      </c>
+      <c r="F21"/>
+      <c r="G21">
+        <v>18.53</v>
+      </c>
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22">
+        <v>27</v>
+      </c>
+      <c r="E22">
+        <v>495.99</v>
+      </c>
+      <c r="F22">
+        <v>18.37</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23">
+        <v>14</v>
+      </c>
+      <c r="E23">
+        <v>236.04</v>
+      </c>
+      <c r="F23">
+        <v>16.86</v>
+      </c>
+      <c r="G23"/>
+      <c r="H23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24">
+        <v>17</v>
+      </c>
+      <c r="E24">
+        <v>98.6</v>
+      </c>
+      <c r="F24">
+        <v>5.8</v>
+      </c>
+      <c r="G24"/>
+      <c r="H24" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>94.61</v>
+      </c>
+      <c r="F25">
+        <v>94.61</v>
+      </c>
+      <c r="G25"/>
+      <c r="H25" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>94.98</v>
+      </c>
+      <c r="F26"/>
+      <c r="G26">
+        <v>94.98</v>
+      </c>
+      <c r="H26" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27">
+        <v>17</v>
+      </c>
+      <c r="E27">
+        <v>102.34</v>
+      </c>
+      <c r="F27"/>
+      <c r="G27">
+        <v>6.02</v>
+      </c>
+      <c r="H27" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28">
+        <v>52</v>
+      </c>
+      <c r="E28">
+        <v>246.48</v>
+      </c>
+      <c r="F28">
+        <v>4.74</v>
+      </c>
+      <c r="G28"/>
+      <c r="H28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>110.14</v>
+      </c>
+      <c r="F29"/>
+      <c r="G29">
+        <v>110.14</v>
+      </c>
+      <c r="H29" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30">
+        <v>28</v>
+      </c>
+      <c r="E30">
+        <v>97.72</v>
+      </c>
+      <c r="F30">
+        <v>3.49</v>
+      </c>
+      <c r="G30"/>
+      <c r="H30" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>109.19</v>
+      </c>
+      <c r="F31"/>
+      <c r="G31">
+        <v>109.19</v>
+      </c>
+      <c r="H31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32">
+        <v>20</v>
+      </c>
+      <c r="E32">
+        <v>114.2</v>
+      </c>
+      <c r="F32"/>
+      <c r="G32">
+        <v>5.71</v>
+      </c>
+      <c r="H32" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33">
+        <v>20</v>
+      </c>
+      <c r="E33">
+        <v>123.8</v>
+      </c>
+      <c r="F33">
+        <v>6.19</v>
+      </c>
+      <c r="G33"/>
+      <c r="H33" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34">
+        <v>52</v>
+      </c>
+      <c r="E34">
+        <v>253.76</v>
+      </c>
+      <c r="F34"/>
+      <c r="G34">
+        <v>4.88</v>
+      </c>
+      <c r="H34" t="s">
+        <v>11</v>
+      </c>
+      <c r="I34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>217.92</v>
+      </c>
+      <c r="F35">
+        <v>108.96</v>
+      </c>
+      <c r="G35"/>
+      <c r="H35" t="s">
+        <v>13</v>
+      </c>
+      <c r="I35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36">
+        <v>28</v>
+      </c>
+      <c r="E36">
+        <v>92.74</v>
+      </c>
+      <c r="F36"/>
+      <c r="G36">
+        <v>3.31</v>
+      </c>
+      <c r="H36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -567,16 +1468,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>38</v>
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -600,14 +1507,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -617,24 +1524,417 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.26953125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B2" s="5">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D2" s="7">
+        <v>99.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>-99.76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="5">
+        <v>0</v>
+      </c>
+      <c r="C5" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D5" s="7">
+        <v>101.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="9">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>-248.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D7" s="7">
+        <v>267.94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="5">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9">
+        <v>-0.03</v>
+      </c>
+      <c r="D8" s="7">
+        <v>500.28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="5">
+        <v>0</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <v>-495.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>-236.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <v>-98.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <v>-94.61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="5">
+        <v>0</v>
+      </c>
+      <c r="C13" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D13" s="7">
+        <v>94.96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="5">
+        <v>0</v>
+      </c>
+      <c r="C14" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D14" s="7">
+        <v>102.32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>-0.02</v>
+      </c>
+      <c r="C15">
+        <v>99.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>-99.76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>-0.02</v>
+      </c>
+      <c r="C18">
+        <v>101.45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>-248.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>-0.02</v>
+      </c>
+      <c r="C20">
+        <v>267.94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>-0.03</v>
+      </c>
+      <c r="C21">
+        <v>500.28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>-495.99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>-236.04</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>-98.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>-94.61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>-0.02</v>
+      </c>
+      <c r="C26">
+        <v>94.96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>-0.02</v>
+      </c>
+      <c r="C27">
+        <v>102.32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>-246.48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>-0.02</v>
+      </c>
+      <c r="C29">
+        <v>110.12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>-97.72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>-0.02</v>
+      </c>
+      <c r="C31">
+        <v>109.17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>-0.02</v>
+      </c>
+      <c r="C32">
+        <v>114.18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>-123.8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>-0.02</v>
+      </c>
+      <c r="C34">
+        <v>253.74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>-217.92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>-0.02</v>
+      </c>
+      <c r="C36">
+        <v>92.72</v>
       </c>
     </row>
   </sheetData>
@@ -660,20 +1960,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>17</v>
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -698,17 +1998,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>21</v>
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -735,23 +2035,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>27</v>
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -769,20 +2069,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>30</v>
+      <c r="A1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -807,17 +2107,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>34</v>
+      <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -829,19 +2129,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
+      <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed parsing issues, and append language to check properly for existing rows
</commit_message>
<xml_diff>
--- a/My-Trading-Journal-Template.xlsx
+++ b/My-Trading-Journal-Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\TradeJournal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DC8744-9427-4FB7-9B7D-7033FA6D1AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77AF5B7-5079-446A-9E8B-73E5A151BEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="97">
   <si>
     <t>Date</t>
   </si>
@@ -107,6 +107,120 @@
   </si>
   <si>
     <t>KTTA</t>
+  </si>
+  <si>
+    <t>09/06/2024</t>
+  </si>
+  <si>
+    <t>WHLR</t>
+  </si>
+  <si>
+    <t>HSDT</t>
+  </si>
+  <si>
+    <t>09/10/2024</t>
+  </si>
+  <si>
+    <t>09/11/2024</t>
+  </si>
+  <si>
+    <t>CNTA</t>
+  </si>
+  <si>
+    <t>CEPU</t>
+  </si>
+  <si>
+    <t>CNEY</t>
+  </si>
+  <si>
+    <t>09/12/2024</t>
+  </si>
+  <si>
+    <t>GV</t>
+  </si>
+  <si>
+    <t>MPW</t>
+  </si>
+  <si>
+    <t>09/13/2024</t>
+  </si>
+  <si>
+    <t>TNON</t>
+  </si>
+  <si>
+    <t>TIL</t>
+  </si>
+  <si>
+    <t>09/16/2024</t>
+  </si>
+  <si>
+    <t>NUVL</t>
+  </si>
+  <si>
+    <t>GNLN</t>
+  </si>
+  <si>
+    <t>09/17/2024</t>
+  </si>
+  <si>
+    <t>IGMS</t>
+  </si>
+  <si>
+    <t>09/18/2024</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>VVOS</t>
+  </si>
+  <si>
+    <t>PRTG</t>
+  </si>
+  <si>
+    <t>09/19/2024</t>
+  </si>
+  <si>
+    <t>APLT</t>
+  </si>
+  <si>
+    <t>BABA</t>
+  </si>
+  <si>
+    <t>INTC</t>
+  </si>
+  <si>
+    <t>09/20/2024</t>
+  </si>
+  <si>
+    <t>GDHG</t>
+  </si>
+  <si>
+    <t>CERO</t>
+  </si>
+  <si>
+    <t>RIVN</t>
+  </si>
+  <si>
+    <t>NBY</t>
+  </si>
+  <si>
+    <t>LUNR</t>
+  </si>
+  <si>
+    <t>09/23/2024</t>
+  </si>
+  <si>
+    <t>KAVL</t>
+  </si>
+  <si>
+    <t>NNE</t>
+  </si>
+  <si>
+    <t>CRSP</t>
+  </si>
+  <si>
+    <t>09/24/2024</t>
   </si>
   <si>
     <t>Stop-Loss Level</t>
@@ -214,8 +328,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00;[Red]#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -269,19 +383,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="46" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -596,8 +708,8 @@
     <col min="2" max="2" width="5.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.453125" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
@@ -616,10 +728,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="8" t="s">
@@ -642,7 +754,7 @@
       <c r="D2">
         <v>86</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="7">
         <v>99.77</v>
       </c>
       <c r="G2" s="9">
@@ -665,10 +777,10 @@
       <c r="D3">
         <v>86</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="7">
         <v>99.76</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="9">
         <v>1.1599999999999999</v>
       </c>
       <c r="H3" t="s">
@@ -688,10 +800,10 @@
       <c r="D4">
         <v>0.34900999999999999</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="7">
         <v>100</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="9">
         <v>286.52</v>
       </c>
       <c r="H4" t="s">
@@ -711,7 +823,7 @@
       <c r="D5">
         <v>0.34900999999999999</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="7">
         <v>101.47</v>
       </c>
       <c r="G5" s="9">
@@ -734,10 +846,10 @@
       <c r="D6">
         <v>8</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="7">
         <v>248.3</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <v>31.04</v>
       </c>
       <c r="H6" t="s">
@@ -757,7 +869,7 @@
       <c r="D7">
         <v>14</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="7">
         <v>267.95999999999998</v>
       </c>
       <c r="G7" s="9">
@@ -780,7 +892,7 @@
       <c r="D8">
         <v>27</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="7">
         <v>500.31</v>
       </c>
       <c r="G8" s="9">
@@ -803,10 +915,10 @@
       <c r="D9">
         <v>27</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="7">
         <v>495.99</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="9">
         <v>18.37</v>
       </c>
       <c r="H9" t="s">
@@ -826,10 +938,10 @@
       <c r="D10">
         <v>14</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="7">
         <v>236.04</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="9">
         <v>16.86</v>
       </c>
       <c r="H10" t="s">
@@ -849,10 +961,10 @@
       <c r="D11">
         <v>17</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="7">
         <v>98.6</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="9">
         <v>5.8</v>
       </c>
       <c r="H11" t="s">
@@ -872,10 +984,10 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="7">
         <v>94.61</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="9">
         <v>94.61</v>
       </c>
       <c r="H12" t="s">
@@ -895,7 +1007,7 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="7">
         <v>94.98</v>
       </c>
       <c r="G13" s="9">
@@ -918,7 +1030,7 @@
       <c r="D14">
         <v>17</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="7">
         <v>102.34</v>
       </c>
       <c r="G14" s="9">
@@ -933,23 +1045,22 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D15">
-        <v>86</v>
-      </c>
-      <c r="E15">
-        <v>99.77</v>
-      </c>
-      <c r="F15"/>
-      <c r="G15">
-        <v>1.1599999999999999</v>
+        <v>52</v>
+      </c>
+      <c r="E15" s="7">
+        <v>246.48</v>
+      </c>
+      <c r="F15" s="9">
+        <v>4.74</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I15" t="s">
         <v>12</v>
@@ -957,23 +1068,22 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D16">
-        <v>86</v>
-      </c>
-      <c r="E16">
-        <v>99.76</v>
-      </c>
-      <c r="F16">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="G16"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="7">
+        <v>110.14</v>
+      </c>
+      <c r="G16" s="9">
+        <v>110.14</v>
+      </c>
       <c r="H16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I16" t="s">
         <v>12</v>
@@ -981,21 +1091,20 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D17">
-        <v>0.34900999999999999</v>
-      </c>
-      <c r="E17">
-        <v>100</v>
-      </c>
-      <c r="F17">
-        <v>286.52</v>
-      </c>
-      <c r="G17"/>
+        <v>28</v>
+      </c>
+      <c r="E17" s="7">
+        <v>97.72</v>
+      </c>
+      <c r="F17" s="9">
+        <v>3.49</v>
+      </c>
       <c r="H17" t="s">
         <v>13</v>
       </c>
@@ -1005,20 +1114,19 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D18">
-        <v>0.34900999999999999</v>
-      </c>
-      <c r="E18">
-        <v>101.47</v>
-      </c>
-      <c r="F18"/>
-      <c r="G18">
-        <v>290.73</v>
+        <v>20</v>
+      </c>
+      <c r="E18" s="7">
+        <v>114.2</v>
+      </c>
+      <c r="G18" s="9">
+        <v>5.71</v>
       </c>
       <c r="H18" t="s">
         <v>11</v>
@@ -1029,21 +1137,20 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D19">
-        <v>8</v>
-      </c>
-      <c r="E19">
-        <v>248.3</v>
-      </c>
-      <c r="F19">
-        <v>31.04</v>
-      </c>
-      <c r="G19"/>
+        <v>20</v>
+      </c>
+      <c r="E19" s="7">
+        <v>123.8</v>
+      </c>
+      <c r="F19" s="9">
+        <v>6.19</v>
+      </c>
       <c r="H19" t="s">
         <v>13</v>
       </c>
@@ -1053,20 +1160,19 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D20">
-        <v>14</v>
-      </c>
-      <c r="E20">
-        <v>267.95999999999998</v>
-      </c>
-      <c r="F20"/>
-      <c r="G20">
-        <v>19.14</v>
+        <v>52</v>
+      </c>
+      <c r="E20" s="7">
+        <v>253.76</v>
+      </c>
+      <c r="G20" s="9">
+        <v>4.88</v>
       </c>
       <c r="H20" t="s">
         <v>11</v>
@@ -1077,23 +1183,22 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D21">
-        <v>27</v>
-      </c>
-      <c r="E21">
-        <v>500.31</v>
-      </c>
-      <c r="F21"/>
-      <c r="G21">
-        <v>18.53</v>
+        <v>2</v>
+      </c>
+      <c r="E21" s="7">
+        <v>217.92</v>
+      </c>
+      <c r="F21" s="9">
+        <v>108.96</v>
       </c>
       <c r="H21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I21" t="s">
         <v>12</v>
@@ -1101,23 +1206,22 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D22">
-        <v>27</v>
-      </c>
-      <c r="E22">
-        <v>495.99</v>
-      </c>
-      <c r="F22">
-        <v>18.37</v>
-      </c>
-      <c r="G22"/>
+        <v>28</v>
+      </c>
+      <c r="E22" s="7">
+        <v>92.74</v>
+      </c>
+      <c r="G22" s="9">
+        <v>3.31</v>
+      </c>
       <c r="H22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I22" t="s">
         <v>12</v>
@@ -1125,23 +1229,23 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D23">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>236.04</v>
-      </c>
-      <c r="F23">
-        <v>16.86</v>
-      </c>
-      <c r="G23"/>
+        <v>8.6</v>
+      </c>
+      <c r="F23"/>
+      <c r="G23">
+        <v>8.6</v>
+      </c>
       <c r="H23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I23" t="s">
         <v>12</v>
@@ -1149,19 +1253,19 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D24">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E24">
-        <v>98.6</v>
+        <v>10</v>
       </c>
       <c r="F24">
-        <v>5.8</v>
+        <v>1</v>
       </c>
       <c r="G24"/>
       <c r="H24" t="s">
@@ -1173,19 +1277,19 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>94.61</v>
+        <v>7.77</v>
       </c>
       <c r="F25">
-        <v>94.61</v>
+        <v>7.77</v>
       </c>
       <c r="G25"/>
       <c r="H25" t="s">
@@ -1197,23 +1301,23 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E26">
-        <v>94.98</v>
-      </c>
-      <c r="F26"/>
-      <c r="G26">
-        <v>94.98</v>
-      </c>
+        <v>93.61</v>
+      </c>
+      <c r="F26">
+        <v>8.51</v>
+      </c>
+      <c r="G26"/>
       <c r="H26" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I26" t="s">
         <v>12</v>
@@ -1221,23 +1325,23 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D27">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E27">
-        <v>102.34</v>
-      </c>
-      <c r="F27"/>
-      <c r="G27">
-        <v>6.02</v>
-      </c>
+        <v>88.26</v>
+      </c>
+      <c r="F27">
+        <v>14.71</v>
+      </c>
+      <c r="G27"/>
       <c r="H27" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I27" t="s">
         <v>12</v>
@@ -1245,23 +1349,23 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D28">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="E28">
-        <v>246.48</v>
-      </c>
-      <c r="F28">
-        <v>4.74</v>
-      </c>
-      <c r="G28"/>
+        <v>253.27</v>
+      </c>
+      <c r="F28"/>
+      <c r="G28">
+        <v>10.130000000000001</v>
+      </c>
       <c r="H28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I28" t="s">
         <v>12</v>
@@ -1269,20 +1373,20 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="E29">
-        <v>110.14</v>
+        <v>121.5</v>
       </c>
       <c r="F29"/>
       <c r="G29">
-        <v>110.14</v>
+        <v>1.35</v>
       </c>
       <c r="H29" t="s">
         <v>11</v>
@@ -1293,23 +1397,23 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D30">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="E30">
-        <v>97.72</v>
-      </c>
-      <c r="F30">
-        <v>3.49</v>
-      </c>
-      <c r="G30"/>
+        <v>85</v>
+      </c>
+      <c r="F30"/>
+      <c r="G30">
+        <v>0.85</v>
+      </c>
       <c r="H30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I30" t="s">
         <v>12</v>
@@ -1317,20 +1421,20 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E31">
-        <v>109.19</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="F31"/>
       <c r="G31">
-        <v>109.19</v>
+        <v>0.97</v>
       </c>
       <c r="H31" t="s">
         <v>11</v>
@@ -1341,23 +1445,23 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D32">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="E32">
-        <v>114.2</v>
-      </c>
-      <c r="F32"/>
-      <c r="G32">
-        <v>5.71</v>
-      </c>
+        <v>116.1</v>
+      </c>
+      <c r="F32">
+        <v>1.29</v>
+      </c>
+      <c r="G32"/>
       <c r="H32" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I32" t="s">
         <v>12</v>
@@ -1365,19 +1469,19 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D33">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E33">
-        <v>123.8</v>
+        <v>10.7</v>
       </c>
       <c r="F33">
-        <v>6.19</v>
+        <v>1.07</v>
       </c>
       <c r="G33"/>
       <c r="H33" t="s">
@@ -1389,23 +1493,23 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D34">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="E34">
-        <v>253.76</v>
-      </c>
-      <c r="F34"/>
-      <c r="G34">
-        <v>4.88</v>
-      </c>
+        <v>249.25</v>
+      </c>
+      <c r="F34">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="G34"/>
       <c r="H34" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I34" t="s">
         <v>12</v>
@@ -1413,19 +1517,19 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D35">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="E35">
-        <v>217.92</v>
+        <v>89</v>
       </c>
       <c r="F35">
-        <v>108.96</v>
+        <v>0.89</v>
       </c>
       <c r="G35"/>
       <c r="H35" t="s">
@@ -1437,25 +1541,1585 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D36">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E36">
-        <v>92.74</v>
+        <v>89.1</v>
       </c>
       <c r="F36"/>
       <c r="G36">
-        <v>3.31</v>
+        <v>14.85</v>
       </c>
       <c r="H36" t="s">
         <v>11</v>
       </c>
       <c r="I36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <v>7.92</v>
+      </c>
+      <c r="F37">
+        <v>3.96</v>
+      </c>
+      <c r="G37"/>
+      <c r="H37" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="F38"/>
+      <c r="G38">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H38" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39">
+        <v>18</v>
+      </c>
+      <c r="E39">
+        <v>98.81</v>
+      </c>
+      <c r="F39">
+        <v>5.49</v>
+      </c>
+      <c r="G39"/>
+      <c r="H39" t="s">
+        <v>13</v>
+      </c>
+      <c r="I39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40">
+        <v>18</v>
+      </c>
+      <c r="E40">
+        <v>101.7</v>
+      </c>
+      <c r="F40"/>
+      <c r="G40">
+        <v>5.65</v>
+      </c>
+      <c r="H40" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41">
+        <v>96.48</v>
+      </c>
+      <c r="F41">
+        <v>12.06</v>
+      </c>
+      <c r="G41"/>
+      <c r="H41" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <v>92.01</v>
+      </c>
+      <c r="F42"/>
+      <c r="G42">
+        <v>11.5</v>
+      </c>
+      <c r="H42" t="s">
+        <v>11</v>
+      </c>
+      <c r="I42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <v>222.14</v>
+      </c>
+      <c r="F43"/>
+      <c r="G43">
+        <v>55.53</v>
+      </c>
+      <c r="H43" t="s">
+        <v>11</v>
+      </c>
+      <c r="I43" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44">
+        <v>4</v>
+      </c>
+      <c r="E44">
+        <v>212</v>
+      </c>
+      <c r="F44">
+        <v>53</v>
+      </c>
+      <c r="G44"/>
+      <c r="H44" t="s">
+        <v>13</v>
+      </c>
+      <c r="I44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45">
+        <v>93.45</v>
+      </c>
+      <c r="F45">
+        <v>31.15</v>
+      </c>
+      <c r="G45"/>
+      <c r="H45" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>102.51</v>
+      </c>
+      <c r="F46">
+        <v>102.51</v>
+      </c>
+      <c r="G46"/>
+      <c r="H46" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47">
+        <v>13</v>
+      </c>
+      <c r="E47">
+        <v>100.88</v>
+      </c>
+      <c r="F47"/>
+      <c r="G47">
+        <v>7.76</v>
+      </c>
+      <c r="H47" t="s">
+        <v>11</v>
+      </c>
+      <c r="I47" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48">
+        <v>45</v>
+      </c>
+      <c r="E48">
+        <v>263.25</v>
+      </c>
+      <c r="F48"/>
+      <c r="G48">
+        <v>5.85</v>
+      </c>
+      <c r="H48" t="s">
+        <v>11</v>
+      </c>
+      <c r="I48" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49">
+        <v>87.33</v>
+      </c>
+      <c r="F49"/>
+      <c r="G49">
+        <v>29.11</v>
+      </c>
+      <c r="H49" t="s">
+        <v>11</v>
+      </c>
+      <c r="I49" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50">
+        <v>45</v>
+      </c>
+      <c r="E50">
+        <v>256.43</v>
+      </c>
+      <c r="F50">
+        <v>5.7</v>
+      </c>
+      <c r="G50"/>
+      <c r="H50" t="s">
+        <v>13</v>
+      </c>
+      <c r="I50" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>109.02</v>
+      </c>
+      <c r="F51"/>
+      <c r="G51">
+        <v>109.02</v>
+      </c>
+      <c r="H51" t="s">
+        <v>11</v>
+      </c>
+      <c r="I51" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52">
+        <v>13</v>
+      </c>
+      <c r="E52">
+        <v>99.97</v>
+      </c>
+      <c r="F52">
+        <v>7.69</v>
+      </c>
+      <c r="G52"/>
+      <c r="H52" t="s">
+        <v>13</v>
+      </c>
+      <c r="I52" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>43</v>
+      </c>
+      <c r="C53" t="s">
+        <v>28</v>
+      </c>
+      <c r="D53">
+        <v>10</v>
+      </c>
+      <c r="E53">
+        <v>7.9</v>
+      </c>
+      <c r="F53"/>
+      <c r="G53">
+        <v>0.79039999999999999</v>
+      </c>
+      <c r="H53" t="s">
+        <v>11</v>
+      </c>
+      <c r="I53" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" t="s">
+        <v>19</v>
+      </c>
+      <c r="D54">
+        <v>8</v>
+      </c>
+      <c r="E54">
+        <v>222.72</v>
+      </c>
+      <c r="F54">
+        <v>27.84</v>
+      </c>
+      <c r="G54"/>
+      <c r="H54" t="s">
+        <v>13</v>
+      </c>
+      <c r="I54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>43</v>
+      </c>
+      <c r="C55" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55">
+        <v>11</v>
+      </c>
+      <c r="E55">
+        <v>99.78</v>
+      </c>
+      <c r="F55"/>
+      <c r="G55">
+        <v>9.07</v>
+      </c>
+      <c r="H55" t="s">
+        <v>11</v>
+      </c>
+      <c r="I55" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>41.2</v>
+      </c>
+      <c r="F56">
+        <v>20.6</v>
+      </c>
+      <c r="G56"/>
+      <c r="H56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I56" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" t="s">
+        <v>44</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>19.510000000000002</v>
+      </c>
+      <c r="F57"/>
+      <c r="G57">
+        <v>19.510000000000002</v>
+      </c>
+      <c r="H57" t="s">
+        <v>11</v>
+      </c>
+      <c r="I57" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>45</v>
+      </c>
+      <c r="C58" t="s">
+        <v>46</v>
+      </c>
+      <c r="D58">
+        <v>8</v>
+      </c>
+      <c r="E58">
+        <v>89.2</v>
+      </c>
+      <c r="F58">
+        <v>11.15</v>
+      </c>
+      <c r="G58"/>
+      <c r="H58" t="s">
+        <v>13</v>
+      </c>
+      <c r="I58" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59">
+        <v>10</v>
+      </c>
+      <c r="E59">
+        <v>49.8</v>
+      </c>
+      <c r="F59">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="G59"/>
+      <c r="H59" t="s">
+        <v>13</v>
+      </c>
+      <c r="I59" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>45</v>
+      </c>
+      <c r="C60" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>16.21</v>
+      </c>
+      <c r="F60"/>
+      <c r="G60">
+        <v>16.21</v>
+      </c>
+      <c r="H60" t="s">
+        <v>11</v>
+      </c>
+      <c r="I60" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61" t="s">
+        <v>48</v>
+      </c>
+      <c r="D61">
+        <v>10</v>
+      </c>
+      <c r="E61">
+        <v>135</v>
+      </c>
+      <c r="F61"/>
+      <c r="G61">
+        <v>13.5</v>
+      </c>
+      <c r="H61" t="s">
+        <v>11</v>
+      </c>
+      <c r="I61" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>45</v>
+      </c>
+      <c r="C62" t="s">
+        <v>48</v>
+      </c>
+      <c r="D62">
+        <v>10</v>
+      </c>
+      <c r="E62">
+        <v>128</v>
+      </c>
+      <c r="F62">
+        <v>12.8</v>
+      </c>
+      <c r="G62"/>
+      <c r="H62" t="s">
+        <v>13</v>
+      </c>
+      <c r="I62" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>45</v>
+      </c>
+      <c r="C63" t="s">
+        <v>47</v>
+      </c>
+      <c r="D63">
+        <v>10</v>
+      </c>
+      <c r="E63">
+        <v>42</v>
+      </c>
+      <c r="F63"/>
+      <c r="G63">
+        <v>4.2</v>
+      </c>
+      <c r="H63" t="s">
+        <v>11</v>
+      </c>
+      <c r="I63" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>45</v>
+      </c>
+      <c r="C64" t="s">
+        <v>19</v>
+      </c>
+      <c r="D64">
+        <v>8</v>
+      </c>
+      <c r="E64">
+        <v>195.44</v>
+      </c>
+      <c r="F64"/>
+      <c r="G64">
+        <v>24.43</v>
+      </c>
+      <c r="H64" t="s">
+        <v>11</v>
+      </c>
+      <c r="I64" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>45</v>
+      </c>
+      <c r="C65" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65">
+        <v>8</v>
+      </c>
+      <c r="E65">
+        <v>234.11</v>
+      </c>
+      <c r="F65"/>
+      <c r="G65">
+        <v>29.26</v>
+      </c>
+      <c r="H65" t="s">
+        <v>11</v>
+      </c>
+      <c r="I65" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>49</v>
+      </c>
+      <c r="C66" t="s">
+        <v>48</v>
+      </c>
+      <c r="D66">
+        <v>24</v>
+      </c>
+      <c r="E66">
+        <v>249.36</v>
+      </c>
+      <c r="F66">
+        <v>10.39</v>
+      </c>
+      <c r="G66"/>
+      <c r="H66" t="s">
+        <v>13</v>
+      </c>
+      <c r="I66" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>49</v>
+      </c>
+      <c r="C67" t="s">
+        <v>50</v>
+      </c>
+      <c r="D67">
+        <v>11</v>
+      </c>
+      <c r="E67">
+        <v>91.52</v>
+      </c>
+      <c r="F67">
+        <v>8.32</v>
+      </c>
+      <c r="G67"/>
+      <c r="H67" t="s">
+        <v>13</v>
+      </c>
+      <c r="I67" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>49</v>
+      </c>
+      <c r="C68" t="s">
+        <v>51</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>88.36</v>
+      </c>
+      <c r="F68"/>
+      <c r="G68">
+        <v>88.36</v>
+      </c>
+      <c r="H68" t="s">
+        <v>11</v>
+      </c>
+      <c r="I68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>49</v>
+      </c>
+      <c r="C69" t="s">
+        <v>52</v>
+      </c>
+      <c r="D69">
+        <v>5</v>
+      </c>
+      <c r="E69">
+        <v>107.05</v>
+      </c>
+      <c r="F69"/>
+      <c r="G69">
+        <v>21.41</v>
+      </c>
+      <c r="H69" t="s">
+        <v>11</v>
+      </c>
+      <c r="I69" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>49</v>
+      </c>
+      <c r="C70" t="s">
+        <v>52</v>
+      </c>
+      <c r="D70">
+        <v>6</v>
+      </c>
+      <c r="E70">
+        <v>129</v>
+      </c>
+      <c r="F70"/>
+      <c r="G70">
+        <v>21.5</v>
+      </c>
+      <c r="H70" t="s">
+        <v>11</v>
+      </c>
+      <c r="I70" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>49</v>
+      </c>
+      <c r="C71" t="s">
+        <v>51</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>87.55</v>
+      </c>
+      <c r="F71">
+        <v>87.55</v>
+      </c>
+      <c r="G71"/>
+      <c r="H71" t="s">
+        <v>13</v>
+      </c>
+      <c r="I71" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>49</v>
+      </c>
+      <c r="C72" t="s">
+        <v>52</v>
+      </c>
+      <c r="D72">
+        <v>11</v>
+      </c>
+      <c r="E72">
+        <v>233.31</v>
+      </c>
+      <c r="F72">
+        <v>21.21</v>
+      </c>
+      <c r="G72"/>
+      <c r="H72" t="s">
+        <v>13</v>
+      </c>
+      <c r="I72" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>49</v>
+      </c>
+      <c r="C73" t="s">
+        <v>48</v>
+      </c>
+      <c r="D73">
+        <v>24</v>
+      </c>
+      <c r="E73">
+        <v>274.93</v>
+      </c>
+      <c r="F73"/>
+      <c r="G73">
+        <v>11.46</v>
+      </c>
+      <c r="H73" t="s">
+        <v>11</v>
+      </c>
+      <c r="I73" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>49</v>
+      </c>
+      <c r="C74" t="s">
+        <v>50</v>
+      </c>
+      <c r="D74">
+        <v>11</v>
+      </c>
+      <c r="E74">
+        <v>93.17</v>
+      </c>
+      <c r="F74"/>
+      <c r="G74">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="H74" t="s">
+        <v>11</v>
+      </c>
+      <c r="I74" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>53</v>
+      </c>
+      <c r="C75" t="s">
+        <v>54</v>
+      </c>
+      <c r="D75">
+        <v>32</v>
+      </c>
+      <c r="E75">
+        <v>99.2</v>
+      </c>
+      <c r="F75">
+        <v>3.1</v>
+      </c>
+      <c r="G75"/>
+      <c r="H75" t="s">
+        <v>13</v>
+      </c>
+      <c r="I75" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>53</v>
+      </c>
+      <c r="C76" t="s">
+        <v>55</v>
+      </c>
+      <c r="D76">
+        <v>780</v>
+      </c>
+      <c r="E76">
+        <v>96.72</v>
+      </c>
+      <c r="F76"/>
+      <c r="G76">
+        <v>0.124</v>
+      </c>
+      <c r="H76" t="s">
+        <v>11</v>
+      </c>
+      <c r="I76" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>53</v>
+      </c>
+      <c r="C77" t="s">
+        <v>55</v>
+      </c>
+      <c r="D77">
+        <v>780</v>
+      </c>
+      <c r="E77">
+        <v>100</v>
+      </c>
+      <c r="F77">
+        <v>0.12820000000000001</v>
+      </c>
+      <c r="G77"/>
+      <c r="H77" t="s">
+        <v>13</v>
+      </c>
+      <c r="I77" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>53</v>
+      </c>
+      <c r="C78" t="s">
+        <v>56</v>
+      </c>
+      <c r="D78">
+        <v>20</v>
+      </c>
+      <c r="E78">
+        <v>241</v>
+      </c>
+      <c r="F78">
+        <v>12.05</v>
+      </c>
+      <c r="G78"/>
+      <c r="H78" t="s">
+        <v>13</v>
+      </c>
+      <c r="I78" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>53</v>
+      </c>
+      <c r="C79" t="s">
+        <v>57</v>
+      </c>
+      <c r="D79">
+        <v>121</v>
+      </c>
+      <c r="E79">
+        <v>96.8</v>
+      </c>
+      <c r="F79"/>
+      <c r="G79">
+        <v>0.8</v>
+      </c>
+      <c r="H79" t="s">
+        <v>11</v>
+      </c>
+      <c r="I79" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>53</v>
+      </c>
+      <c r="C80" t="s">
+        <v>56</v>
+      </c>
+      <c r="D80">
+        <v>20</v>
+      </c>
+      <c r="E80">
+        <v>237.8</v>
+      </c>
+      <c r="F80"/>
+      <c r="G80">
+        <v>11.89</v>
+      </c>
+      <c r="H80" t="s">
+        <v>11</v>
+      </c>
+      <c r="I80" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>53</v>
+      </c>
+      <c r="C81" t="s">
+        <v>54</v>
+      </c>
+      <c r="D81">
+        <v>32</v>
+      </c>
+      <c r="E81">
+        <v>94.08</v>
+      </c>
+      <c r="F81"/>
+      <c r="G81">
+        <v>2.94</v>
+      </c>
+      <c r="H81" t="s">
+        <v>11</v>
+      </c>
+      <c r="I81" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>53</v>
+      </c>
+      <c r="C82" t="s">
+        <v>58</v>
+      </c>
+      <c r="D82">
+        <v>11</v>
+      </c>
+      <c r="E82">
+        <v>99.55</v>
+      </c>
+      <c r="F82">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="G82"/>
+      <c r="H82" t="s">
+        <v>13</v>
+      </c>
+      <c r="I82" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>53</v>
+      </c>
+      <c r="C83" t="s">
+        <v>57</v>
+      </c>
+      <c r="D83">
+        <v>121</v>
+      </c>
+      <c r="E83">
+        <v>105.27</v>
+      </c>
+      <c r="F83">
+        <v>0.87</v>
+      </c>
+      <c r="G83"/>
+      <c r="H83" t="s">
+        <v>13</v>
+      </c>
+      <c r="I83" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>53</v>
+      </c>
+      <c r="C84" t="s">
+        <v>58</v>
+      </c>
+      <c r="D84">
+        <v>11</v>
+      </c>
+      <c r="E84">
+        <v>101.97</v>
+      </c>
+      <c r="F84"/>
+      <c r="G84">
+        <v>9.27</v>
+      </c>
+      <c r="H84" t="s">
+        <v>11</v>
+      </c>
+      <c r="I84" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>59</v>
+      </c>
+      <c r="C85" t="s">
+        <v>60</v>
+      </c>
+      <c r="D85">
+        <v>50</v>
+      </c>
+      <c r="E85">
+        <v>85.5</v>
+      </c>
+      <c r="F85"/>
+      <c r="G85">
+        <v>1.71</v>
+      </c>
+      <c r="H85" t="s">
+        <v>11</v>
+      </c>
+      <c r="I85" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>59</v>
+      </c>
+      <c r="C86" t="s">
+        <v>61</v>
+      </c>
+      <c r="D86">
+        <v>7</v>
+      </c>
+      <c r="E86">
+        <v>94.92</v>
+      </c>
+      <c r="F86"/>
+      <c r="G86">
+        <v>13.56</v>
+      </c>
+      <c r="H86" t="s">
+        <v>11</v>
+      </c>
+      <c r="I86" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>59</v>
+      </c>
+      <c r="C87" t="s">
+        <v>22</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>94.48</v>
+      </c>
+      <c r="F87">
+        <v>94.48</v>
+      </c>
+      <c r="G87"/>
+      <c r="H87" t="s">
+        <v>13</v>
+      </c>
+      <c r="I87" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>59</v>
+      </c>
+      <c r="C88" t="s">
+        <v>52</v>
+      </c>
+      <c r="D88">
+        <v>2</v>
+      </c>
+      <c r="E88">
+        <v>44.46</v>
+      </c>
+      <c r="F88">
+        <v>22.23</v>
+      </c>
+      <c r="G88"/>
+      <c r="H88" t="s">
+        <v>13</v>
+      </c>
+      <c r="I88" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>59</v>
+      </c>
+      <c r="C89" t="s">
+        <v>61</v>
+      </c>
+      <c r="D89">
+        <v>17</v>
+      </c>
+      <c r="E89">
+        <v>240.38</v>
+      </c>
+      <c r="F89"/>
+      <c r="G89">
+        <v>14.14</v>
+      </c>
+      <c r="H89" t="s">
+        <v>11</v>
+      </c>
+      <c r="I89" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>59</v>
+      </c>
+      <c r="C90" t="s">
+        <v>61</v>
+      </c>
+      <c r="D90">
+        <v>10</v>
+      </c>
+      <c r="E90">
+        <v>141</v>
+      </c>
+      <c r="F90">
+        <v>14.1</v>
+      </c>
+      <c r="G90"/>
+      <c r="H90" t="s">
+        <v>13</v>
+      </c>
+      <c r="I90" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>59</v>
+      </c>
+      <c r="C91" t="s">
+        <v>61</v>
+      </c>
+      <c r="D91">
+        <v>7</v>
+      </c>
+      <c r="E91">
+        <v>92.82</v>
+      </c>
+      <c r="F91">
+        <v>13.26</v>
+      </c>
+      <c r="G91"/>
+      <c r="H91" t="s">
+        <v>13</v>
+      </c>
+      <c r="I91" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>59</v>
+      </c>
+      <c r="C92" t="s">
+        <v>62</v>
+      </c>
+      <c r="D92">
+        <v>2</v>
+      </c>
+      <c r="E92">
+        <v>95.72</v>
+      </c>
+      <c r="F92">
+        <v>47.86</v>
+      </c>
+      <c r="G92"/>
+      <c r="H92" t="s">
+        <v>13</v>
+      </c>
+      <c r="I92" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>59</v>
+      </c>
+      <c r="C93" t="s">
+        <v>39</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>66.5</v>
+      </c>
+      <c r="F93"/>
+      <c r="G93">
+        <v>66.5</v>
+      </c>
+      <c r="H93" t="s">
+        <v>11</v>
+      </c>
+      <c r="I93" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>59</v>
+      </c>
+      <c r="C94" t="s">
+        <v>61</v>
+      </c>
+      <c r="D94">
+        <v>10</v>
+      </c>
+      <c r="E94">
+        <v>144</v>
+      </c>
+      <c r="F94"/>
+      <c r="G94">
+        <v>14.4</v>
+      </c>
+      <c r="H94" t="s">
+        <v>11</v>
+      </c>
+      <c r="I94" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>59</v>
+      </c>
+      <c r="C95" t="s">
+        <v>22</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95">
+        <v>93.05</v>
+      </c>
+      <c r="F95"/>
+      <c r="G95">
+        <v>93.05</v>
+      </c>
+      <c r="H95" t="s">
+        <v>11</v>
+      </c>
+      <c r="I95" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>59</v>
+      </c>
+      <c r="C96" t="s">
+        <v>52</v>
+      </c>
+      <c r="D96">
+        <v>2</v>
+      </c>
+      <c r="E96">
+        <v>44.5</v>
+      </c>
+      <c r="F96"/>
+      <c r="G96">
+        <v>22.25</v>
+      </c>
+      <c r="H96" t="s">
+        <v>11</v>
+      </c>
+      <c r="I96" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>59</v>
+      </c>
+      <c r="C97" t="s">
+        <v>61</v>
+      </c>
+      <c r="D97">
+        <v>17</v>
+      </c>
+      <c r="E97">
+        <v>238</v>
+      </c>
+      <c r="F97">
+        <v>14</v>
+      </c>
+      <c r="G97"/>
+      <c r="H97" t="s">
+        <v>13</v>
+      </c>
+      <c r="I97" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>59</v>
+      </c>
+      <c r="C98" t="s">
+        <v>39</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>68.34</v>
+      </c>
+      <c r="F98">
+        <v>68.34</v>
+      </c>
+      <c r="G98"/>
+      <c r="H98" t="s">
+        <v>13</v>
+      </c>
+      <c r="I98" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>59</v>
+      </c>
+      <c r="C99" t="s">
+        <v>60</v>
+      </c>
+      <c r="D99">
+        <v>50</v>
+      </c>
+      <c r="E99">
+        <v>81.95</v>
+      </c>
+      <c r="F99">
+        <v>1.64</v>
+      </c>
+      <c r="G99"/>
+      <c r="H99" t="s">
+        <v>13</v>
+      </c>
+      <c r="I99" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>63</v>
+      </c>
+      <c r="C100" t="s">
+        <v>21</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+      <c r="E100">
+        <v>8.25</v>
+      </c>
+      <c r="F100"/>
+      <c r="G100">
+        <v>8.25</v>
+      </c>
+      <c r="H100" t="s">
+        <v>11</v>
+      </c>
+      <c r="I100" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>63</v>
+      </c>
+      <c r="C101" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101">
+        <v>7.78</v>
+      </c>
+      <c r="F101">
+        <v>7.78</v>
+      </c>
+      <c r="G101"/>
+      <c r="H101" t="s">
+        <v>13</v>
+      </c>
+      <c r="I101" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1480,10 +3144,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1508,13 +3172,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1524,421 +3188,1216 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F103" sqref="F103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.26953125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>30</v>
+      <c r="A1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>32</v>
+        <v>69</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="5">
+      <c r="B2" s="9">
         <v>0</v>
       </c>
       <c r="C2" s="9">
         <v>-0.02</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="9">
         <v>99.75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="5">
+      <c r="B3" s="9">
         <v>0</v>
       </c>
       <c r="C3" s="9">
         <v>0</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="9">
         <v>-99.76</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="5">
+      <c r="B4" s="9">
         <v>0</v>
       </c>
       <c r="C4" s="9">
         <v>0</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="9">
         <v>-100</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="5">
+      <c r="B5" s="9">
         <v>0</v>
       </c>
       <c r="C5" s="9">
         <v>-0.02</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="9">
         <v>101.45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="5">
+      <c r="B6" s="9">
         <v>0</v>
       </c>
       <c r="C6" s="9">
         <v>0</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="9">
         <v>-248.3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="5">
+      <c r="B7" s="9">
         <v>0</v>
       </c>
       <c r="C7" s="9">
         <v>-0.02</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="9">
         <v>267.94</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B8" s="5">
+      <c r="B8" s="9">
         <v>0</v>
       </c>
       <c r="C8" s="9">
         <v>-0.03</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="9">
         <v>500.28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="5">
+      <c r="B9" s="9">
         <v>0</v>
       </c>
       <c r="C9" s="9">
         <v>0</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="9">
         <v>-495.99</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B10" s="5">
+      <c r="B10" s="9">
         <v>0</v>
       </c>
       <c r="C10" s="9">
         <v>0</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="9">
         <v>-236.04</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="5">
+      <c r="B11" s="9">
         <v>0</v>
       </c>
       <c r="C11" s="9">
         <v>0</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="9">
         <v>-98.6</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="5">
+      <c r="B12" s="9">
         <v>0</v>
       </c>
       <c r="C12" s="9">
         <v>0</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="9">
         <v>-94.61</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="5">
+      <c r="B13" s="9">
         <v>0</v>
       </c>
       <c r="C13" s="9">
         <v>-0.02</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="9">
         <v>94.96</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B14" s="5">
+      <c r="B14" s="9">
         <v>0</v>
       </c>
       <c r="C14" s="9">
         <v>-0.02</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="9">
         <v>102.32</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15">
+      <c r="B15" s="9">
+        <v>0</v>
+      </c>
+      <c r="C15" s="9">
+        <v>0</v>
+      </c>
+      <c r="D15" s="9">
+        <v>-246.48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B16" s="9">
+        <v>0</v>
+      </c>
+      <c r="C16" s="9">
         <v>-0.02</v>
       </c>
-      <c r="C15">
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>-99.76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
+      <c r="D16" s="9">
+        <v>110.12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="9">
+        <v>0</v>
+      </c>
+      <c r="C17" s="9">
+        <v>0</v>
+      </c>
+      <c r="D17" s="9">
+        <v>-97.72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="9">
+        <v>0</v>
+      </c>
+      <c r="C18" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D18" s="9">
+        <v>114.18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="9">
+        <v>0</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0</v>
+      </c>
+      <c r="D19" s="9">
+        <v>-123.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="9">
+        <v>0</v>
+      </c>
+      <c r="C20" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D20" s="9">
+        <v>253.74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="9">
+        <v>0</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>-217.92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B22" s="9">
+        <v>0</v>
+      </c>
+      <c r="C22" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D22" s="9">
+        <v>92.72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23"/>
+      <c r="B23" s="9">
+        <v>0</v>
+      </c>
+      <c r="C23" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D23" s="9">
+        <v>8.58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24"/>
+      <c r="B24" s="9">
+        <v>0</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0</v>
+      </c>
+      <c r="D24" s="9">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25"/>
+      <c r="B25" s="9">
+        <v>0</v>
+      </c>
+      <c r="C25" s="9">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9">
+        <v>-7.77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26"/>
+      <c r="B26" s="9">
+        <v>0</v>
+      </c>
+      <c r="C26" s="9">
+        <v>0</v>
+      </c>
+      <c r="D26" s="9">
+        <v>-93.61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27"/>
+      <c r="B27" s="9">
+        <v>0</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0</v>
+      </c>
+      <c r="D27" s="9">
+        <v>-88.26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28"/>
+      <c r="B28" s="9">
+        <v>0</v>
+      </c>
+      <c r="C28" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D28" s="9">
+        <v>253.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29"/>
+      <c r="B29" s="9">
+        <v>0</v>
+      </c>
+      <c r="C29" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D29" s="9">
+        <v>121.48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30"/>
+      <c r="B30" s="9">
+        <v>0</v>
+      </c>
+      <c r="C30" s="9">
+        <v>-0.03</v>
+      </c>
+      <c r="D30" s="9">
+        <v>84.97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31"/>
+      <c r="B31" s="9">
+        <v>0</v>
+      </c>
+      <c r="C31" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D31" s="9">
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32"/>
+      <c r="B32" s="9">
+        <v>0</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0</v>
+      </c>
+      <c r="D32" s="9">
+        <v>-116.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33"/>
+      <c r="B33" s="9">
+        <v>0</v>
+      </c>
+      <c r="C33" s="9">
+        <v>0</v>
+      </c>
+      <c r="D33" s="9">
+        <v>-10.7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34"/>
+      <c r="B34" s="9">
+        <v>0</v>
+      </c>
+      <c r="C34" s="9">
+        <v>0</v>
+      </c>
+      <c r="D34" s="9">
+        <v>-249.25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35"/>
+      <c r="B35" s="9">
+        <v>0</v>
+      </c>
+      <c r="C35" s="9">
+        <v>0</v>
+      </c>
+      <c r="D35" s="9">
+        <v>-89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36"/>
+      <c r="B36" s="9">
+        <v>0</v>
+      </c>
+      <c r="C36" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D36" s="9">
+        <v>89.08</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37"/>
+      <c r="B37" s="9">
+        <v>0</v>
+      </c>
+      <c r="C37" s="9">
+        <v>0</v>
+      </c>
+      <c r="D37" s="9">
+        <v>-7.92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38"/>
+      <c r="B38" s="9">
+        <v>0</v>
+      </c>
+      <c r="C38" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D38" s="9">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39"/>
+      <c r="B39" s="9">
+        <v>0</v>
+      </c>
+      <c r="C39" s="9">
+        <v>0</v>
+      </c>
+      <c r="D39" s="9">
+        <v>-98.81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40"/>
+      <c r="B40" s="9">
+        <v>0</v>
+      </c>
+      <c r="C40" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D40" s="9">
+        <v>101.68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41"/>
+      <c r="B41" s="9">
+        <v>0</v>
+      </c>
+      <c r="C41" s="9">
+        <v>0</v>
+      </c>
+      <c r="D41" s="9">
+        <v>-96.48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42"/>
+      <c r="B42" s="9">
+        <v>0</v>
+      </c>
+      <c r="C42" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D42" s="9">
+        <v>91.99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43"/>
+      <c r="B43" s="9">
+        <v>0</v>
+      </c>
+      <c r="C43" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D43" s="9">
+        <v>222.12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44"/>
+      <c r="B44" s="9">
+        <v>0</v>
+      </c>
+      <c r="C44" s="9">
+        <v>0</v>
+      </c>
+      <c r="D44" s="9">
+        <v>-212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45"/>
+      <c r="B45" s="9">
+        <v>0</v>
+      </c>
+      <c r="C45" s="9">
+        <v>0</v>
+      </c>
+      <c r="D45" s="9">
+        <v>-93.45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46"/>
+      <c r="B46" s="9">
+        <v>0</v>
+      </c>
+      <c r="C46" s="9">
+        <v>0</v>
+      </c>
+      <c r="D46" s="9">
+        <v>-102.51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47"/>
+      <c r="B47" s="9">
+        <v>0</v>
+      </c>
+      <c r="C47" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D47" s="9">
+        <v>100.86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48"/>
+      <c r="B48" s="9">
+        <v>0</v>
+      </c>
+      <c r="C48" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D48" s="9">
+        <v>263.23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49"/>
+      <c r="B49" s="9">
+        <v>0</v>
+      </c>
+      <c r="C49" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D49" s="9">
+        <v>87.31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50"/>
+      <c r="B50" s="9">
+        <v>0</v>
+      </c>
+      <c r="C50" s="9">
+        <v>0</v>
+      </c>
+      <c r="D50" s="9">
+        <v>-256.43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51"/>
+      <c r="B51" s="9">
+        <v>0</v>
+      </c>
+      <c r="C51" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D51" s="9">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52"/>
+      <c r="B52" s="9">
+        <v>0</v>
+      </c>
+      <c r="C52" s="9">
+        <v>0</v>
+      </c>
+      <c r="D52" s="9">
+        <v>-99.97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53"/>
+      <c r="B53" s="9">
+        <v>0</v>
+      </c>
+      <c r="C53" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D53" s="9">
+        <v>7.88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54"/>
+      <c r="B54" s="9">
+        <v>0</v>
+      </c>
+      <c r="C54" s="9">
+        <v>0</v>
+      </c>
+      <c r="D54" s="9">
+        <v>-222.72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55"/>
+      <c r="B55" s="9">
+        <v>0</v>
+      </c>
+      <c r="C55" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D55" s="9">
+        <v>99.76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56"/>
+      <c r="B56" s="9">
+        <v>0</v>
+      </c>
+      <c r="C56" s="9">
+        <v>0</v>
+      </c>
+      <c r="D56" s="9">
+        <v>-41.2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57"/>
+      <c r="B57" s="9">
+        <v>0</v>
+      </c>
+      <c r="C57" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D57" s="9">
+        <v>19.489999999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58"/>
+      <c r="B58" s="9">
+        <v>0</v>
+      </c>
+      <c r="C58" s="9">
+        <v>0</v>
+      </c>
+      <c r="D58" s="9">
+        <v>-89.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59"/>
+      <c r="B59" s="9">
+        <v>0</v>
+      </c>
+      <c r="C59" s="9">
+        <v>0</v>
+      </c>
+      <c r="D59" s="9">
+        <v>-49.8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60"/>
+      <c r="B60" s="9">
+        <v>0</v>
+      </c>
+      <c r="C60" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D60" s="9">
+        <v>16.190000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61"/>
+      <c r="B61" s="9">
+        <v>0</v>
+      </c>
+      <c r="C61" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D61" s="9">
+        <v>134.97999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62"/>
+      <c r="B62" s="9">
+        <v>0</v>
+      </c>
+      <c r="C62" s="9">
+        <v>0</v>
+      </c>
+      <c r="D62" s="9">
+        <v>-128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63"/>
+      <c r="B63" s="9">
+        <v>0</v>
+      </c>
+      <c r="C63" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D63" s="9">
+        <v>41.98</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64"/>
+      <c r="B64" s="9">
+        <v>0</v>
+      </c>
+      <c r="C64" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D64" s="9">
+        <v>195.42</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65"/>
+      <c r="B65" s="9">
+        <v>0</v>
+      </c>
+      <c r="C65" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D65" s="9">
+        <v>234.09</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66"/>
+      <c r="B66" s="9">
+        <v>0</v>
+      </c>
+      <c r="C66" s="9">
+        <v>0</v>
+      </c>
+      <c r="D66" s="9">
+        <v>-249.36</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67"/>
+      <c r="B67" s="9">
+        <v>0</v>
+      </c>
+      <c r="C67" s="9">
+        <v>0</v>
+      </c>
+      <c r="D67" s="9">
+        <v>-91.52</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68"/>
+      <c r="B68" s="9">
+        <v>0</v>
+      </c>
+      <c r="C68" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D68" s="9">
+        <v>88.34</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69"/>
+      <c r="B69" s="9">
+        <v>0</v>
+      </c>
+      <c r="C69" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D69" s="9">
+        <v>107.03</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70"/>
+      <c r="B70" s="9">
+        <v>0</v>
+      </c>
+      <c r="C70" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D70" s="9">
+        <v>128.97999999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71"/>
+      <c r="B71" s="9">
+        <v>0</v>
+      </c>
+      <c r="C71" s="9">
+        <v>0</v>
+      </c>
+      <c r="D71" s="9">
+        <v>-87.55</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72"/>
+      <c r="B72" s="9">
+        <v>0</v>
+      </c>
+      <c r="C72" s="9">
+        <v>0</v>
+      </c>
+      <c r="D72" s="9">
+        <v>-233.31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73"/>
+      <c r="B73" s="9">
+        <v>0</v>
+      </c>
+      <c r="C73" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D73" s="9">
+        <v>274.91000000000003</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74"/>
+      <c r="B74" s="9">
+        <v>0</v>
+      </c>
+      <c r="C74" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D74" s="9">
+        <v>93.15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75"/>
+      <c r="B75" s="9">
+        <v>0</v>
+      </c>
+      <c r="C75" s="9">
+        <v>0</v>
+      </c>
+      <c r="D75" s="9">
+        <v>-99.2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76"/>
+      <c r="B76" s="9">
+        <v>0</v>
+      </c>
+      <c r="C76" s="9">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="D76" s="9">
+        <v>96.58</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77"/>
+      <c r="B77" s="9">
+        <v>0</v>
+      </c>
+      <c r="C77" s="9">
+        <v>0</v>
+      </c>
+      <c r="D77" s="9">
         <v>-100</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="B18">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78"/>
+      <c r="B78" s="9">
+        <v>0</v>
+      </c>
+      <c r="C78" s="9">
+        <v>0</v>
+      </c>
+      <c r="D78" s="9">
+        <v>-241</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79"/>
+      <c r="B79" s="9">
+        <v>0</v>
+      </c>
+      <c r="C79" s="9">
+        <v>-0.03</v>
+      </c>
+      <c r="D79" s="9">
+        <v>96.77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80"/>
+      <c r="B80" s="9">
+        <v>0</v>
+      </c>
+      <c r="C80" s="9">
         <v>-0.02</v>
       </c>
-      <c r="C18">
-        <v>101.45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>-248.3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20">
+      <c r="D80" s="9">
+        <v>237.78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81"/>
+      <c r="B81" s="9">
+        <v>0</v>
+      </c>
+      <c r="C81" s="9">
         <v>-0.02</v>
       </c>
-      <c r="C20">
-        <v>267.94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="B21">
-        <v>-0.03</v>
-      </c>
-      <c r="C21">
-        <v>500.28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>0</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>-495.99</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>0</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>-236.04</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>0</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>-98.6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>0</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>-94.61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26">
-        <v>0</v>
-      </c>
-      <c r="B26">
+      <c r="D81" s="9">
+        <v>94.06</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82"/>
+      <c r="B82" s="9">
+        <v>0</v>
+      </c>
+      <c r="C82" s="9">
+        <v>0</v>
+      </c>
+      <c r="D82" s="9">
+        <v>-99.55</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83"/>
+      <c r="B83" s="9">
+        <v>0</v>
+      </c>
+      <c r="C83" s="9">
+        <v>0</v>
+      </c>
+      <c r="D83" s="9">
+        <v>-105.27</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84"/>
+      <c r="B84" s="9">
+        <v>0</v>
+      </c>
+      <c r="C84" s="9">
         <v>-0.02</v>
       </c>
-      <c r="C26">
-        <v>94.96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27">
-        <v>0</v>
-      </c>
-      <c r="B27">
+      <c r="D84" s="9">
+        <v>101.95</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85"/>
+      <c r="B85" s="9">
+        <v>0</v>
+      </c>
+      <c r="C85" s="9">
         <v>-0.02</v>
       </c>
-      <c r="C27">
-        <v>102.32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>0</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>-246.48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>0</v>
-      </c>
-      <c r="B29">
+      <c r="D85" s="9">
+        <v>85.48</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86"/>
+      <c r="B86" s="9">
+        <v>0</v>
+      </c>
+      <c r="C86" s="9">
         <v>-0.02</v>
       </c>
-      <c r="C29">
-        <v>110.12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>0</v>
-      </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <v>-97.72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>0</v>
-      </c>
-      <c r="B31">
+      <c r="D86" s="9">
+        <v>94.9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87"/>
+      <c r="B87" s="9">
+        <v>0</v>
+      </c>
+      <c r="C87" s="9">
+        <v>0</v>
+      </c>
+      <c r="D87" s="9">
+        <v>-94.48</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88"/>
+      <c r="B88" s="9">
+        <v>0</v>
+      </c>
+      <c r="C88" s="9">
+        <v>0</v>
+      </c>
+      <c r="D88" s="9">
+        <v>-44.46</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89"/>
+      <c r="B89" s="9">
+        <v>0</v>
+      </c>
+      <c r="C89" s="9">
         <v>-0.02</v>
       </c>
-      <c r="C31">
-        <v>109.17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>0</v>
-      </c>
-      <c r="B32">
+      <c r="D89" s="9">
+        <v>240.36</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90"/>
+      <c r="B90" s="9">
+        <v>0</v>
+      </c>
+      <c r="C90" s="9">
+        <v>0</v>
+      </c>
+      <c r="D90" s="9">
+        <v>-141</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91"/>
+      <c r="B91" s="9">
+        <v>0</v>
+      </c>
+      <c r="C91" s="9">
+        <v>0</v>
+      </c>
+      <c r="D91" s="9">
+        <v>-92.82</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A92"/>
+      <c r="B92" s="9">
+        <v>0</v>
+      </c>
+      <c r="C92" s="9">
+        <v>0</v>
+      </c>
+      <c r="D92" s="9">
+        <v>-95.72</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93"/>
+      <c r="B93" s="9">
+        <v>0</v>
+      </c>
+      <c r="C93" s="9">
         <v>-0.02</v>
       </c>
-      <c r="C32">
-        <v>114.18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>0</v>
-      </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>-123.8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>0</v>
-      </c>
-      <c r="B34">
+      <c r="D93" s="9">
+        <v>66.48</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A94"/>
+      <c r="B94" s="9">
+        <v>0</v>
+      </c>
+      <c r="C94" s="9">
         <v>-0.02</v>
       </c>
-      <c r="C34">
-        <v>253.74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>0</v>
-      </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <v>-217.92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>0</v>
-      </c>
-      <c r="B36">
+      <c r="D94" s="9">
+        <v>143.97999999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A95"/>
+      <c r="B95" s="9">
+        <v>0</v>
+      </c>
+      <c r="C95" s="9">
         <v>-0.02</v>
       </c>
-      <c r="C36">
-        <v>92.72</v>
+      <c r="D95" s="9">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A96"/>
+      <c r="B96" s="9">
+        <v>0</v>
+      </c>
+      <c r="C96" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D96" s="9">
+        <v>44.48</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A97"/>
+      <c r="B97" s="9">
+        <v>0</v>
+      </c>
+      <c r="C97" s="9">
+        <v>0</v>
+      </c>
+      <c r="D97" s="9">
+        <v>-238</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A98"/>
+      <c r="B98" s="9">
+        <v>0</v>
+      </c>
+      <c r="C98" s="9">
+        <v>0</v>
+      </c>
+      <c r="D98" s="9">
+        <v>-68.34</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A99"/>
+      <c r="B99" s="9">
+        <v>0</v>
+      </c>
+      <c r="C99" s="9">
+        <v>0</v>
+      </c>
+      <c r="D99" s="9">
+        <v>-81.95</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A100"/>
+      <c r="B100" s="9">
+        <v>0</v>
+      </c>
+      <c r="C100" s="9">
+        <v>-0.02</v>
+      </c>
+      <c r="D100" s="9">
+        <v>8.23</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A101"/>
+      <c r="B101" s="9">
+        <v>0</v>
+      </c>
+      <c r="C101" s="9">
+        <v>0</v>
+      </c>
+      <c r="D101" s="9">
+        <v>-7.78</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1961,19 +4420,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1999,16 +4458,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2036,22 +4495,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2076,13 +4535,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2108,16 +4567,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2141,10 +4600,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>